<commit_message>
Incomplete invariant analysis for Horner's rule
Committed and uploaded so available to continue analysis.
</commit_message>
<xml_diff>
--- a/Documents/Horner's Rule.xlsx
+++ b/Documents/Horner's Rule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>i</t>
   </si>
@@ -1527,6 +1527,344 @@
         <scheme val="minor"/>
       </rPr>
       <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Analysis of Invariant:</t>
+  </si>
+  <si>
+    <t>Initialisation:</t>
+  </si>
+  <si>
+    <t>Maintenance:</t>
+  </si>
+  <si>
+    <t>Termination:</t>
+  </si>
+  <si>
+    <t>Condition:</t>
+  </si>
+  <si>
+    <t>On initialisation and before the first loop runs, y = 0.
+As i is initialised to n, the expression n-(i+1) evaluates to -1.  Therefore the invariant summation is already past the upper bound it is supposed to run to (0 &gt; -1) and no iterations are performed.  Therefore the invariant sums to 0, matching the initial value of y.
+From this we can conclude that the invariant holds on initialisation.</t>
+  </si>
+  <si>
+    <r>
+      <t>The invariant must hold true for the start of each calculation loop of the more easily computable (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Θ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(n)) form:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">y = 0
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> i=n </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>downto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0
+    y = a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + x.y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+which must be proven to ultimately evaluate to:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">          n
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">y = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Σ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="16"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="16"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+          k=0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>As the calculation loop runs, i decreases by 1 each time and thus the number of terms the invariant is expected to sum (n-(i+1)) increases by 1 each time.  This is consistent with the addition of a new term (a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) with each iteration of the calculation loop.  This constant a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> corresponds to the iteration k=0, which is present whenever the invariant loop is checked  - the constant is initially multiplied only by x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (i.e. 1).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The previous value of y is then multiplied by x and added to the constant, meaning that:
+Because the number of times a term has been passed through the loop determines the power x is raised to, the term introduced earliest (a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> where k = n-(i+1)) is raised to the highest power.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
     </r>
   </si>
 </sst>
@@ -1534,10 +1872,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1682,6 +2027,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="16"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="16"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1770,23 +2176,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -1798,17 +2204,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -1862,11 +2277,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2148,10 +2575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2198,7 +2625,7 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -2213,12 +2640,12 @@
       <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="I3" s="11"/>
+      <c r="F3" s="16"/>
+      <c r="I3" s="14"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1">
@@ -2233,15 +2660,15 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="12"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:11" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1">
@@ -2256,10 +2683,10 @@
       <c r="E5" s="1">
         <v>-1</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
     </row>
     <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -2303,179 +2730,268 @@
       <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="21">
         <v>3</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="22" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="30">
         <v>0</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="34">
         <v>0</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="22" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
-      <c r="C9" s="18">
+      <c r="C9" s="21">
         <v>2</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="22" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="9"/>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="20">
         <v>0</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="34">
         <v>2</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="J9" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
-      <c r="C10" s="21">
+      <c r="C10" s="24">
         <v>1</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="25" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="20">
         <v>0</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="22" t="s">
+      <c r="K10" s="25" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="9"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="17">
+      <c r="G11" s="20">
         <v>1</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="32"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="24"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="21">
+      <c r="C12" s="24">
         <v>0</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="25" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="20">
         <v>0</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="28" t="s">
+      <c r="J12" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="K12" s="25" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="17">
+      <c r="G13" s="20">
         <v>1</v>
       </c>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="26"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="26"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="29"/>
     </row>
     <row r="14" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="17">
+      <c r="G14" s="20">
         <v>2</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="24"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="24"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+    </row>
+    <row r="17" spans="1:11" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+    </row>
+    <row r="18" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+    </row>
+    <row r="19" spans="1:11" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+    </row>
+    <row r="20" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="23">
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:K19"/>
+    <mergeCell ref="C20:K20"/>
+    <mergeCell ref="C17:K17"/>
+    <mergeCell ref="A17:A20"/>
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="J12:J14"/>
     <mergeCell ref="K12:K14"/>
     <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:K16"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="D12:D14"/>

</xml_diff>

<commit_message>
"Good enough" completion of Horner's Rule proof
Might revisit to clear up a bit but basically covers off a lot of the
required logic.
</commit_message>
<xml_diff>
--- a/Documents/Horner's Rule.xlsx
+++ b/Documents/Horner's Rule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>i</t>
   </si>
@@ -1757,7 +1757,97 @@
   </si>
   <si>
     <r>
-      <t>As the calculation loop runs, i decreases by 1 each time and thus the number of terms the invariant is expected to sum (n-(i+1)) increases by 1 each time.  This is consistent with the addition of a new term (a</t>
+      <t xml:space="preserve">The final completed calculation loop has value of i = 0.  On loop termination, it is in effect at the start of a loop for i = -1.  Hence for the invariant which we know to hold on maintenance, it has the value equal to:
+        n
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">y = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="26"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Σ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+          k=0
+which is demonstrably equivalent to the original polynomial we are trying to solve.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>As the calculation loop runs, i decreases by 1 each time and thus the number of terms the invariant is expected to sum (that is, n-(i+1) ) increases by 1 each time.  This is consistent with the addition of a new term (a</t>
     </r>
     <r>
       <rPr>
@@ -1821,24 +1911,22 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (i.e. 1).
+Each term already existing from the previous iteration of the calculation loop is multiplied by x (i.e. it's power of x is raised by 1), which is consistent with the fact that the maximum value of k is increased each time, and also the fact that the constant a is assigned a different power in each check of the invariant, offset by one due to its index (k+i+1) being dependent on the value of i.
 </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The previous value of y is then multiplied by x and added to the constant, meaning that:
-Because the number of times a term has been passed through the loop determines the power x is raised to, the term introduced earliest (a</t>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Because the number of times a term has been passed through the loop determines the power x is raised to, the term introduced earliest (a</t>
     </r>
     <r>
       <rPr>
         <vertAlign val="subscript"/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1848,23 +1936,11 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> where k = n-(i+1)) is raised to the highest power.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> where k = n-(i+1) ) is raised to the highest power, subsequent terms are raised to a power less by one for each term in turn.</t>
     </r>
   </si>
 </sst>
@@ -1872,17 +1948,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2081,9 +2150,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <vertAlign val="subscript"/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2176,24 +2257,106 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2204,96 +2367,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2577,8 +2655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:K19"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2598,19 +2676,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -2625,27 +2703,27 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="I3" s="14"/>
+      <c r="F3" s="9"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1">
@@ -2660,15 +2738,15 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="15"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:11" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1">
@@ -2683,16 +2761,16 @@
       <c r="E5" s="1">
         <v>-1</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2724,273 +2802,269 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="14">
         <v>3</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="17">
         <v>0</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="18">
         <v>0</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="21">
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="14">
         <v>2</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="19" t="s">
+      <c r="E9" s="37"/>
+      <c r="F9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="13">
         <v>0</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="34">
+      <c r="I9" s="18">
         <v>2</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="22" t="s">
+      <c r="K9" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="24">
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="33">
         <v>1</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="37"/>
+      <c r="F10" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="13">
         <v>0</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="31" t="s">
+      <c r="J10" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="25" t="s">
+      <c r="K10" s="26" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="26"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="27"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="20">
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="13">
         <v>1</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="35"/>
-      <c r="J11" s="32"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="25"/>
       <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="24">
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="33">
         <v>0</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="8" t="s">
+      <c r="E12" s="37"/>
+      <c r="F12" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="13">
         <v>0</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="31" t="s">
+      <c r="J12" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="25" t="s">
+      <c r="K12" s="26" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="48.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="28"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="29"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="20">
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="13">
         <v>1</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="17" t="s">
         <v>41</v>
       </c>
       <c r="I13" s="29"/>
-      <c r="J13" s="33"/>
+      <c r="J13" s="28"/>
       <c r="K13" s="29"/>
     </row>
     <row r="14" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="26"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="27"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="20">
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="13">
         <v>2</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="H14" s="17" t="s">
         <v>42</v>
       </c>
       <c r="I14" s="27"/>
-      <c r="J14" s="32"/>
+      <c r="J14" s="25"/>
       <c r="K14" s="27"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
     </row>
     <row r="17" spans="1:11" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
     </row>
     <row r="18" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="39" t="s">
+      <c r="A18" s="22"/>
+      <c r="B18" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="39" t="s">
+    <row r="19" spans="1:11" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+    </row>
+    <row r="20" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-    </row>
-    <row r="20" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:K19"/>
-    <mergeCell ref="C20:K20"/>
-    <mergeCell ref="C17:K17"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="B8:B14"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="A16:K16"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="C12:C14"/>
@@ -3000,10 +3074,16 @@
     <mergeCell ref="I12:I14"/>
     <mergeCell ref="A8:A14"/>
     <mergeCell ref="E8:E14"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="B8:B14"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:K19"/>
+    <mergeCell ref="C20:K20"/>
+    <mergeCell ref="C17:K17"/>
+    <mergeCell ref="A17:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>